<commit_message>
Finalizando mesa da aula_11 POO (Herança, classe e abstract)
</commit_message>
<xml_diff>
--- a/Turma 6/Testing l/Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]/A7S [Técnica de Testes]/Caso de Teste [Tipo de Testes].xlsx
+++ b/Turma 6/Testing l/Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]/A7S [Técnica de Testes]/Caso de Teste [Tipo de Testes].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Desktop\CTD\Turma 6\Testing l\Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]\A7S [Técnica de Testes]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E8FFAB-1275-4E3C-9A34-DD6A4626C1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF693B70-2404-4CAC-B593-BAD9BC1F07D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4F8A38D9-B9C1-42D6-AEB2-396C93C0EC4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F8A38D9-B9C1-42D6-AEB2-396C93C0EC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Nome do Tester:</t>
   </si>
@@ -270,12 +270,30 @@
   <si>
     <t>Sétido dia gratuido</t>
   </si>
+  <si>
+    <t>Testes dinâmicos</t>
+  </si>
+  <si>
+    <t>Testes estáticos</t>
+  </si>
+  <si>
+    <t>É realizado com o código "rodando", tendo interação.</t>
+  </si>
+  <si>
+    <t>É realizado em documentos / casos de teste</t>
+  </si>
+  <si>
+    <t>O teste é realizado na detecção do defeito(bug) com o programa / sistema em funcionamento</t>
+  </si>
+  <si>
+    <t>O teste pode ser realizado nas primeiras etapas do projeto, como no planejamento.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,18 +353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -365,6 +371,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -586,80 +599,82 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,16 +1057,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7072082B-18AF-40DB-A58A-DF7A3E5CFFC7}">
-  <dimension ref="A1:Z41"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
@@ -1156,7 +1171,7 @@
       <c r="A9" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1168,302 +1183,349 @@
       <c r="A10" s="13">
         <v>2</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:26" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:26" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="26">
         <v>3</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="26" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="18"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="27"/>
     </row>
     <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="26">
         <v>4</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="27"/>
     </row>
     <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="26">
         <v>5</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="18"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="27"/>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="36" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="36" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="A26" s="28">
         <v>6</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="18"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="A28" s="28">
         <v>7</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="28"/>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
+      <c r="A30" s="28">
         <v>8</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21" t="s">
+      <c r="B30" s="29"/>
+      <c r="C30" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="33">
+      <c r="B32" s="20">
         <v>1</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="20">
         <v>2</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D32" s="20">
         <v>3</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="E35" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="40"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="39"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+      <c r="A39" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="41"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="40"/>
+      <c r="B41" s="41"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="40"/>
+      <c r="B42" s="41"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
+  <mergeCells count="37">
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
@@ -1473,14 +1535,18 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <conditionalFormatting sqref="E9 E11:E12 E10:F10">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">

</xml_diff>